<commit_message>
Global Southern and Irminger SUMO
Added GS01SUMO D2 cal and Integration
Updated GI01SUMO cal for D1 and D2
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GI01SUMO_00002.xlsx
+++ b/deployment/Omaha_Cal_Info_GI01SUMO_00002.xlsx
@@ -1623,7 +1623,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="410">
+  <cellStyleXfs count="411">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -2034,6 +2034,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2416,7 +2417,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="410">
+  <cellStyles count="411">
     <cellStyle name="Comma 2" xfId="72"/>
     <cellStyle name="Comma 2 2" xfId="100"/>
     <cellStyle name="Comma 2 2 2" xfId="101"/>
@@ -2721,6 +2722,7 @@
     <cellStyle name="Normal 15" xfId="3"/>
     <cellStyle name="Normal 15 2" xfId="98"/>
     <cellStyle name="Normal 16" xfId="99"/>
+    <cellStyle name="Normal 18" xfId="410"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 2 2" xfId="6"/>
     <cellStyle name="Normal 2 2 2" xfId="19"/>
@@ -3290,8 +3292,8 @@
   <dimension ref="A1:AMM361"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I186" sqref="I186"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added CC_ct_depth for DOSTA
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GI01SUMO_00002.xlsx
+++ b/deployment/Omaha_Cal_Info_GI01SUMO_00002.xlsx
@@ -3296,7 +3296,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A338" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G250" sqref="G250"/>
+      <selection pane="bottomLeft" activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6157,7 +6157,9 @@
       <c r="G32" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29">
+        <v>1</v>
+      </c>
       <c r="I32" s="55"/>
       <c r="J32" s="50"/>
       <c r="K32" s="131"/>
@@ -6283,7 +6285,9 @@
       <c r="G37" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="H37" s="29"/>
+      <c r="H37" s="29">
+        <v>12</v>
+      </c>
       <c r="I37" s="55"/>
       <c r="J37" s="50"/>
       <c r="K37" s="131"/>
@@ -6409,7 +6413,9 @@
       <c r="G42" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="H42" s="29"/>
+      <c r="H42" s="29">
+        <v>40</v>
+      </c>
       <c r="I42" s="51"/>
       <c r="J42" s="50"/>
       <c r="K42" s="131"/>
@@ -6528,7 +6534,9 @@
       <c r="G47" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="H47" s="29"/>
+      <c r="H47" s="29">
+        <v>80</v>
+      </c>
       <c r="I47" s="51"/>
       <c r="K47" s="131"/>
     </row>
@@ -6645,7 +6653,9 @@
       <c r="G52" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="H52" s="29"/>
+      <c r="H52" s="29">
+        <v>130</v>
+      </c>
       <c r="I52" s="51"/>
       <c r="K52" s="131"/>
     </row>

</xml_diff>

<commit_message>
Issue #11089 - Correct reference designator for several entries
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GI01SUMO_00002.xlsx
+++ b/deployment/Omaha_Cal_Info_GI01SUMO_00002.xlsx
@@ -476,9 +476,6 @@
     </r>
   </si>
   <si>
-    <t>GI01SUMO-RID16-07-NUTNRB000</t>
-  </si>
-  <si>
     <t>CC_upper_wavelength_limit_for_spectra_fit</t>
   </si>
   <si>
@@ -507,6 +504,9 @@
   </si>
   <si>
     <t>[34, 27, 47, 39, 47, 45, 40, 34, 36, 38, 28, 33, 35, 59, 145, 377, 982, 2075, 3646, 5586, 7657, 9664, 11441, 12898, 14060, 14940, 15665, 16327, 16929, 17733, 18611, 19653, 20921, 22413, 24154, 26197, 28434, 30861, 33432, 36007, 38367, 40359, 41846, 42705, 42873, 42335, 41295, 39916, 38338, 36746, 35317, 34105, 33151, 32489, 32110, 32003, 32133, 32437, 29025, 32245, 34623, 35633, 36819, 38147, 39575, 41027, 42432, 43782, 44945, 45744, 46177, 46148, 45615, 44610, 43117, 41274, 39191, 36953, 34717, 32565, 30521, 28608, 26941, 25418, 24084, 22917, 21917, 21099, 20414, 19841, 19407, 19145, 18929, 18867, 18899, 19036, 19282, 19607, 19991, 20441, 20929, 21393, 21869, 22305, 22638, 22885, 22991, 22934, 22738, 22387, 21915, 21307, 20615, 19848, 19085, 18296, 17553, 16846, 16176, 15561, 15021, 14530, 14118, 13769, 13483, 13254, 13099, 12977, 12924, 12889, 12900, 12953, 13041, 13159, 13314, 13469, 13681, 13885, 14130, 14371, 14641, 14899, 15182, 15437, 15706, 15951, 16209, 16415, 16590, 16734, 16841, 16904, 16920, 16865, 16771, 16617, 16397, 16160, 15696, 15507, 15194, 14829, 14439, 14049, 13649, 13251, 12850, 12468, 12085, 11664, 11251, 10862, 10497, 10118, 9781, 9487, 9194, 8931, 8696, 8487, 8305, 8137, 7992, 7854, 7709, 7588, 7464, 7360, 7245, 7135, 7021, 6917, 6828, 6745, 6690, 6609, 6562, 6508, 6462, 6407, 6385, 6361, 6331, 6312, 6284, 6277, 6254, 6243, 6234, 6229, 6198, 6177, 6180, 6142, 6105, 6082, 6045, 5990, 5948, 5904, 5837, 5760, 5690, 5571, 5452, 5345, 5219, 5108, 5000, 4887, 4790, 4689, 4609, 4526, 4444, 4357, 4278, 4173, 4071, 3967, 3873, 3772, 3707, 3622, 3561, 3490, 3436, 3398, 3353, 3294, 3271, 3234, 3198, 3170, 3090, 3090]</t>
+  </si>
+  <si>
+    <t>GI01SUMO-RID16-07-NUTNRB000</t>
   </si>
   <si>
     <t>A01143</t>
@@ -6032,8 +6032,8 @@
       <c r="V62" s="6"/>
     </row>
     <row r="63" ht="15" customHeight="1">
-      <c r="A63" t="s" s="61">
-        <v>93</v>
+      <c r="A63" t="s" s="33">
+        <v>89</v>
       </c>
       <c r="B63" t="s" s="34">
         <v>12</v>
@@ -6051,7 +6051,7 @@
         <v>274</v>
       </c>
       <c r="G63" t="s" s="98">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H63" s="99">
         <v>240</v>
@@ -6074,8 +6074,8 @@
       <c r="V63" s="6"/>
     </row>
     <row r="64" ht="15" customHeight="1">
-      <c r="A64" t="s" s="61">
-        <v>93</v>
+      <c r="A64" t="s" s="33">
+        <v>89</v>
       </c>
       <c r="B64" t="s" s="34">
         <v>12</v>
@@ -6093,7 +6093,7 @@
         <v>274</v>
       </c>
       <c r="G64" t="s" s="98">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H64" s="101">
         <v>20.02</v>
@@ -6114,8 +6114,8 @@
       <c r="V64" s="6"/>
     </row>
     <row r="65" ht="15" customHeight="1">
-      <c r="A65" t="s" s="61">
-        <v>93</v>
+      <c r="A65" t="s" s="33">
+        <v>89</v>
       </c>
       <c r="B65" t="s" s="34">
         <v>12</v>
@@ -6133,10 +6133,10 @@
         <v>274</v>
       </c>
       <c r="G65" t="s" s="98">
+        <v>95</v>
+      </c>
+      <c r="H65" t="s" s="55">
         <v>96</v>
-      </c>
-      <c r="H65" t="s" s="55">
-        <v>97</v>
       </c>
       <c r="I65" s="79"/>
       <c r="J65" s="52"/>
@@ -6154,8 +6154,8 @@
       <c r="V65" s="6"/>
     </row>
     <row r="66" ht="15" customHeight="1">
-      <c r="A66" t="s" s="61">
-        <v>93</v>
+      <c r="A66" t="s" s="33">
+        <v>89</v>
       </c>
       <c r="B66" t="s" s="34">
         <v>12</v>
@@ -6173,10 +6173,10 @@
         <v>274</v>
       </c>
       <c r="G66" t="s" s="98">
+        <v>97</v>
+      </c>
+      <c r="H66" t="s" s="55">
         <v>98</v>
-      </c>
-      <c r="H66" t="s" s="55">
-        <v>99</v>
       </c>
       <c r="I66" s="79"/>
       <c r="J66" s="52"/>
@@ -6194,8 +6194,8 @@
       <c r="V66" s="6"/>
     </row>
     <row r="67" ht="15" customHeight="1">
-      <c r="A67" t="s" s="61">
-        <v>93</v>
+      <c r="A67" t="s" s="33">
+        <v>89</v>
       </c>
       <c r="B67" t="s" s="34">
         <v>12</v>
@@ -6213,10 +6213,10 @@
         <v>274</v>
       </c>
       <c r="G67" t="s" s="98">
+        <v>99</v>
+      </c>
+      <c r="H67" t="s" s="55">
         <v>100</v>
-      </c>
-      <c r="H67" t="s" s="55">
-        <v>101</v>
       </c>
       <c r="I67" s="79"/>
       <c r="J67" s="52"/>
@@ -6234,8 +6234,8 @@
       <c r="V67" s="6"/>
     </row>
     <row r="68" ht="15" customHeight="1">
-      <c r="A68" t="s" s="61">
-        <v>93</v>
+      <c r="A68" t="s" s="33">
+        <v>89</v>
       </c>
       <c r="B68" t="s" s="34">
         <v>12</v>
@@ -6253,10 +6253,10 @@
         <v>274</v>
       </c>
       <c r="G68" t="s" s="98">
+        <v>101</v>
+      </c>
+      <c r="H68" t="s" s="55">
         <v>102</v>
-      </c>
-      <c r="H68" t="s" s="55">
-        <v>103</v>
       </c>
       <c r="I68" s="79"/>
       <c r="J68" s="52"/>
@@ -6299,7 +6299,7 @@
     </row>
     <row r="70" ht="28" customHeight="1">
       <c r="A70" t="s" s="33">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B70" t="s" s="34">
         <v>12</v>
@@ -6341,7 +6341,7 @@
     </row>
     <row r="71" ht="15" customHeight="1">
       <c r="A71" t="s" s="61">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B71" t="s" s="34">
         <v>12</v>
@@ -6359,7 +6359,7 @@
         <v>271</v>
       </c>
       <c r="G71" t="s" s="98">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H71" s="99">
         <v>240</v>
@@ -6383,7 +6383,7 @@
     </row>
     <row r="72" ht="15" customHeight="1">
       <c r="A72" t="s" s="61">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B72" t="s" s="34">
         <v>12</v>
@@ -6401,7 +6401,7 @@
         <v>271</v>
       </c>
       <c r="G72" t="s" s="98">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H72" s="101">
         <v>19.98</v>
@@ -6423,7 +6423,7 @@
     </row>
     <row r="73" ht="15" customHeight="1">
       <c r="A73" t="s" s="61">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B73" t="s" s="34">
         <v>12</v>
@@ -6441,7 +6441,7 @@
         <v>271</v>
       </c>
       <c r="G73" t="s" s="98">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H73" t="s" s="55">
         <v>106</v>
@@ -6463,7 +6463,7 @@
     </row>
     <row r="74" ht="15" customHeight="1">
       <c r="A74" t="s" s="61">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B74" t="s" s="34">
         <v>12</v>
@@ -6481,7 +6481,7 @@
         <v>271</v>
       </c>
       <c r="G74" t="s" s="98">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H74" t="s" s="55">
         <v>107</v>
@@ -6503,7 +6503,7 @@
     </row>
     <row r="75" ht="15" customHeight="1">
       <c r="A75" t="s" s="61">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B75" t="s" s="34">
         <v>12</v>
@@ -6521,7 +6521,7 @@
         <v>271</v>
       </c>
       <c r="G75" t="s" s="98">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H75" t="s" s="55">
         <v>108</v>
@@ -6543,7 +6543,7 @@
     </row>
     <row r="76" ht="15" customHeight="1">
       <c r="A76" t="s" s="61">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B76" t="s" s="34">
         <v>12</v>
@@ -6561,7 +6561,7 @@
         <v>271</v>
       </c>
       <c r="G76" t="s" s="98">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H76" t="s" s="55">
         <v>109</v>

</xml_diff>